<commit_message>
Se agrego funcionalidad para borrar datos de cache al cerrar sesion
</commit_message>
<xml_diff>
--- a/resumen_movimiento_cuenta.xlsx
+++ b/resumen_movimiento_cuenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\pruebas\lacteos-doel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0628AF-98A1-4E00-90D6-64F2D3AF7856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B2209-AA1F-446C-876F-A85224D69DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,10 +677,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="[Blue]#,##0.00;[Red]\(#,##0.00\);[Black]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,6 +694,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -726,17 +735,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1037,15 +1050,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1099,7 +1113,7 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>2847.8</v>
       </c>
       <c r="F2">
@@ -1140,7 +1154,7 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>16864.28</v>
       </c>
       <c r="F3">
@@ -1156,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>98.9</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1165,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>16864.28</v>
+        <v>16765.38</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1181,7 +1195,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>4563.3599999999997</v>
       </c>
       <c r="F4">
@@ -1222,7 +1236,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>1620</v>
       </c>
       <c r="F5">
@@ -1263,7 +1277,7 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>800.18</v>
       </c>
       <c r="F6">
@@ -1304,7 +1318,7 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>83.229999999999905</v>
       </c>
       <c r="F7">
@@ -1345,7 +1359,7 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>1883.84</v>
       </c>
       <c r="F8">
@@ -1386,7 +1400,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>1714</v>
       </c>
       <c r="F9">
@@ -1427,7 +1441,7 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>943.79</v>
       </c>
       <c r="F10">
@@ -1468,7 +1482,7 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>2101.3200000000002</v>
       </c>
       <c r="F11">
@@ -1509,7 +1523,7 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>564.79999999999995</v>
       </c>
       <c r="F12">
@@ -1550,7 +1564,7 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>3976.85</v>
       </c>
       <c r="F13">
@@ -1591,8 +1605,8 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14">
-        <v>1106.1199999999999</v>
+      <c r="E14" s="4">
+        <v>1105.77</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1607,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>106.02</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1616,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1106.1199999999999</v>
+        <v>999.75</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1632,7 +1646,7 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>947.28</v>
       </c>
       <c r="F15">
@@ -1673,7 +1687,7 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>859.56</v>
       </c>
       <c r="F16">
@@ -1714,7 +1728,7 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>-0.46</v>
       </c>
       <c r="F17">
@@ -1755,7 +1769,7 @@
       <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>10.69000000000001</v>
       </c>
       <c r="F18">
@@ -1796,7 +1810,7 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>183.48</v>
       </c>
       <c r="F19">
@@ -1837,7 +1851,7 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>4846.1499999999996</v>
       </c>
       <c r="F20">
@@ -1878,7 +1892,7 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>1055.25</v>
       </c>
       <c r="F21">
@@ -1919,7 +1933,7 @@
       <c r="D22" t="s">
         <v>14</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>78.41</v>
       </c>
       <c r="F22">
@@ -1960,7 +1974,7 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>368.74</v>
       </c>
       <c r="F23">
@@ -2001,7 +2015,7 @@
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>236.95</v>
       </c>
       <c r="F24">
@@ -2042,7 +2056,7 @@
       <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>14402.57</v>
       </c>
       <c r="F25">
@@ -2083,7 +2097,7 @@
       <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>9156.2100000000028</v>
       </c>
       <c r="F26">
@@ -2124,7 +2138,7 @@
       <c r="D27" t="s">
         <v>14</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>2540.7600000000002</v>
       </c>
       <c r="F27">
@@ -2165,7 +2179,7 @@
       <c r="D28" t="s">
         <v>14</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>2031.85</v>
       </c>
       <c r="F28">
@@ -2206,7 +2220,7 @@
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>4990.32</v>
       </c>
       <c r="F29">
@@ -2247,7 +2261,7 @@
       <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <v>1269.5</v>
       </c>
       <c r="F30">
@@ -2288,7 +2302,7 @@
       <c r="D31" t="s">
         <v>14</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="4">
         <v>1071.42</v>
       </c>
       <c r="F31">
@@ -2329,7 +2343,7 @@
       <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>2724.05</v>
       </c>
       <c r="F32">
@@ -2370,7 +2384,7 @@
       <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="4">
         <v>307.26</v>
       </c>
       <c r="F33">
@@ -2411,7 +2425,7 @@
       <c r="D34" t="s">
         <v>14</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>909</v>
       </c>
       <c r="F34">
@@ -2452,7 +2466,7 @@
       <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="4">
         <v>304.67999999999978</v>
       </c>
       <c r="F35">
@@ -2493,7 +2507,7 @@
       <c r="D36" t="s">
         <v>14</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="4">
         <v>228.47</v>
       </c>
       <c r="F36">
@@ -2534,7 +2548,7 @@
       <c r="D37" t="s">
         <v>14</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="4">
         <v>159.66999999999999</v>
       </c>
       <c r="F37">
@@ -2575,7 +2589,7 @@
       <c r="D38" t="s">
         <v>14</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>1660.53</v>
       </c>
       <c r="F38">
@@ -2616,7 +2630,7 @@
       <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="4">
         <v>-1085.8400000000011</v>
       </c>
       <c r="F39">
@@ -2632,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1049.51</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2641,7 +2655,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <v>-1085.8399999999999</v>
+        <v>-2135.35</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2657,7 +2671,7 @@
       <c r="D40" t="s">
         <v>14</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="4">
         <v>569.36</v>
       </c>
       <c r="F40">
@@ -2698,7 +2712,7 @@
       <c r="D41" t="s">
         <v>14</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>-2095.84</v>
       </c>
       <c r="F41">
@@ -2739,7 +2753,7 @@
       <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="4">
         <v>489.18</v>
       </c>
       <c r="F42">
@@ -2780,7 +2794,7 @@
       <c r="D43" t="s">
         <v>14</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="4">
         <v>-187.8600000000001</v>
       </c>
       <c r="F43">
@@ -2821,7 +2835,7 @@
       <c r="D44" t="s">
         <v>14</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="4">
         <v>53.76</v>
       </c>
       <c r="F44">
@@ -2862,7 +2876,7 @@
       <c r="D45" t="s">
         <v>14</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="4">
         <v>-0.02</v>
       </c>
       <c r="F45">
@@ -2903,7 +2917,7 @@
       <c r="D46" t="s">
         <v>14</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="4">
         <v>683</v>
       </c>
       <c r="F46">
@@ -2944,7 +2958,7 @@
       <c r="D47" t="s">
         <v>14</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="4">
         <v>394.73999999999933</v>
       </c>
       <c r="F47">
@@ -2985,7 +2999,7 @@
       <c r="D48" t="s">
         <v>14</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="4">
         <v>6262.21</v>
       </c>
       <c r="F48">
@@ -3026,7 +3040,7 @@
       <c r="D49" t="s">
         <v>14</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="4">
         <v>3661.02</v>
       </c>
       <c r="F49">
@@ -3067,7 +3081,7 @@
       <c r="D50" t="s">
         <v>14</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="4">
         <v>639.80000000000007</v>
       </c>
       <c r="F50">
@@ -3108,7 +3122,7 @@
       <c r="D51" t="s">
         <v>14</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="4">
         <v>1770.84</v>
       </c>
       <c r="F51">
@@ -3149,7 +3163,7 @@
       <c r="D52" t="s">
         <v>14</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="4">
         <v>127.52</v>
       </c>
       <c r="F52">
@@ -3190,7 +3204,7 @@
       <c r="D53" t="s">
         <v>14</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="4">
         <v>6142.72</v>
       </c>
       <c r="F53">
@@ -3231,7 +3245,7 @@
       <c r="D54" t="s">
         <v>14</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="4">
         <v>-692.71999999999991</v>
       </c>
       <c r="F54">
@@ -3247,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -3256,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="2">
-        <v>-692.72</v>
+        <v>-998.72</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3272,7 +3286,7 @@
       <c r="D55" t="s">
         <v>14</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="4">
         <v>258.99000000000012</v>
       </c>
       <c r="F55">
@@ -3313,7 +3327,7 @@
       <c r="D56" t="s">
         <v>14</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="4">
         <v>349.97</v>
       </c>
       <c r="F56">
@@ -3354,7 +3368,7 @@
       <c r="D57" t="s">
         <v>14</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="4">
         <v>571.19999999999993</v>
       </c>
       <c r="F57">
@@ -3395,7 +3409,7 @@
       <c r="D58" t="s">
         <v>14</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="4">
         <v>2703.54</v>
       </c>
       <c r="F58">
@@ -3436,7 +3450,7 @@
       <c r="D59" t="s">
         <v>14</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="4">
         <v>218.42</v>
       </c>
       <c r="F59">
@@ -3477,7 +3491,7 @@
       <c r="D60" t="s">
         <v>14</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="4">
         <v>68.539999999999793</v>
       </c>
       <c r="F60">
@@ -3518,7 +3532,7 @@
       <c r="D61" t="s">
         <v>14</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="4">
         <v>46.5</v>
       </c>
       <c r="F61">
@@ -3559,7 +3573,7 @@
       <c r="D62" t="s">
         <v>14</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="4">
         <v>628.66</v>
       </c>
       <c r="F62">
@@ -3600,7 +3614,7 @@
       <c r="D63" t="s">
         <v>14</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="4">
         <v>6065.4</v>
       </c>
       <c r="F63">
@@ -3641,7 +3655,7 @@
       <c r="D64" t="s">
         <v>14</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="4">
         <v>8.27</v>
       </c>
       <c r="F64">
@@ -3682,7 +3696,7 @@
       <c r="D65" t="s">
         <v>14</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="4">
         <v>3152.91</v>
       </c>
       <c r="F65">
@@ -3723,7 +3737,7 @@
       <c r="D66" t="s">
         <v>14</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="4">
         <v>7385.7500000000036</v>
       </c>
       <c r="F66">
@@ -3739,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>0</v>
+        <v>2197.8000000000002</v>
       </c>
       <c r="K66">
         <v>0</v>
@@ -3748,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="2">
-        <v>7385.75</v>
+        <v>5187.95</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3764,7 +3778,7 @@
       <c r="D67" t="s">
         <v>14</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="4">
         <v>1464.44</v>
       </c>
       <c r="F67">
@@ -3805,7 +3819,7 @@
       <c r="D68" t="s">
         <v>14</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="4">
         <v>-7519.579999999999</v>
       </c>
       <c r="F68">
@@ -3815,13 +3829,13 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>99.61</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>416.77</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -3830,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="2">
-        <v>-7519.58</v>
+        <v>-8035.96</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3846,7 +3860,7 @@
       <c r="D69" t="s">
         <v>14</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="4">
         <v>765.75</v>
       </c>
       <c r="F69">
@@ -3887,7 +3901,7 @@
       <c r="D70" t="s">
         <v>14</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="4">
         <v>508.61000000000041</v>
       </c>
       <c r="F70">
@@ -3928,7 +3942,7 @@
       <c r="D71" t="s">
         <v>14</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="4">
         <v>-4366.3500000000004</v>
       </c>
       <c r="F71">
@@ -3969,7 +3983,7 @@
       <c r="D72" t="s">
         <v>14</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="4">
         <v>332.51</v>
       </c>
       <c r="F72">
@@ -4010,7 +4024,7 @@
       <c r="D73" t="s">
         <v>14</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="4">
         <v>-0.45</v>
       </c>
       <c r="F73">
@@ -4051,7 +4065,7 @@
       <c r="D74" t="s">
         <v>14</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="4">
         <v>69.7</v>
       </c>
       <c r="F74">
@@ -4092,7 +4106,7 @@
       <c r="D75" t="s">
         <v>14</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="4">
         <v>-45.32</v>
       </c>
       <c r="F75">
@@ -4133,7 +4147,7 @@
       <c r="D76" t="s">
         <v>14</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="4">
         <v>15773.34</v>
       </c>
       <c r="F76">
@@ -4174,7 +4188,7 @@
       <c r="D77" t="s">
         <v>14</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="4">
         <v>146.16999999999999</v>
       </c>
       <c r="F77">
@@ -4215,7 +4229,7 @@
       <c r="D78" t="s">
         <v>14</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="4">
         <v>15630.76</v>
       </c>
       <c r="F78">
@@ -4256,7 +4270,7 @@
       <c r="D79" t="s">
         <v>14</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="4">
         <v>5474.67</v>
       </c>
       <c r="F79">
@@ -4297,7 +4311,7 @@
       <c r="D80" t="s">
         <v>14</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="4">
         <v>200.92</v>
       </c>
       <c r="F80">
@@ -4338,7 +4352,7 @@
       <c r="D81" t="s">
         <v>14</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="4">
         <v>664.13</v>
       </c>
       <c r="F81">
@@ -4379,7 +4393,7 @@
       <c r="D82" t="s">
         <v>14</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="4">
         <v>-0.01</v>
       </c>
       <c r="F82">
@@ -4420,7 +4434,7 @@
       <c r="D83" t="s">
         <v>14</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="4">
         <v>3.01</v>
       </c>
       <c r="F83">
@@ -4461,7 +4475,7 @@
       <c r="D84" t="s">
         <v>14</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="4">
         <v>-0.04</v>
       </c>
       <c r="F84">
@@ -4502,7 +4516,7 @@
       <c r="D85" t="s">
         <v>14</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="4">
         <v>17878.04</v>
       </c>
       <c r="F85">
@@ -4543,7 +4557,7 @@
       <c r="D86" t="s">
         <v>14</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="4">
         <v>460.68</v>
       </c>
       <c r="F86">
@@ -4584,7 +4598,7 @@
       <c r="D87" t="s">
         <v>14</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="4">
         <v>399.98</v>
       </c>
       <c r="F87">
@@ -4625,8 +4639,8 @@
       <c r="D88" t="s">
         <v>14</v>
       </c>
-      <c r="E88">
-        <v>1095.9699999999989</v>
+      <c r="E88" s="4">
+        <v>1091.79</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -4650,7 +4664,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="2">
-        <v>1095.97</v>
+        <v>1091.79</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4666,7 +4680,7 @@
       <c r="D89" t="s">
         <v>14</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="4">
         <v>243.14</v>
       </c>
       <c r="F89">
@@ -4707,7 +4721,7 @@
       <c r="D90" t="s">
         <v>14</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="4">
         <v>1162.33</v>
       </c>
       <c r="F90">
@@ -4748,7 +4762,7 @@
       <c r="D91" t="s">
         <v>14</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="4">
         <v>8032.94</v>
       </c>
       <c r="F91">
@@ -4789,7 +4803,7 @@
       <c r="D92" t="s">
         <v>14</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="4">
         <v>261.20999999999998</v>
       </c>
       <c r="F92">
@@ -4830,7 +4844,7 @@
       <c r="D93" t="s">
         <v>14</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="4">
         <v>24.050000000000072</v>
       </c>
       <c r="F93">
@@ -4871,7 +4885,7 @@
       <c r="D94" t="s">
         <v>14</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="4">
         <v>3714.63</v>
       </c>
       <c r="F94">
@@ -4912,7 +4926,7 @@
       <c r="D95" t="s">
         <v>14</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="4">
         <v>240.98</v>
       </c>
       <c r="F95">
@@ -4953,7 +4967,7 @@
       <c r="D96" t="s">
         <v>14</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="4">
         <v>127.77</v>
       </c>
       <c r="F96">
@@ -4981,7 +4995,7 @@
         <v>127.77</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>206</v>
       </c>
@@ -4994,7 +5008,7 @@
       <c r="D97" t="s">
         <v>14</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="4">
         <v>234.759999999999</v>
       </c>
       <c r="F97">
@@ -5022,7 +5036,7 @@
         <v>234.76</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>208</v>
       </c>
@@ -5035,7 +5049,7 @@
       <c r="D98" t="s">
         <v>14</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="4">
         <v>32396.41</v>
       </c>
       <c r="F98">
@@ -5063,7 +5077,7 @@
         <v>32396.41</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>210</v>
       </c>
@@ -5076,7 +5090,7 @@
       <c r="D99" t="s">
         <v>14</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="4">
         <v>785.53999999999985</v>
       </c>
       <c r="F99">
@@ -5104,7 +5118,7 @@
         <v>785.54</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>214</v>
       </c>
@@ -5117,7 +5131,7 @@
       <c r="D100" t="s">
         <v>14</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="4">
         <v>79.42</v>
       </c>
       <c r="F100">
@@ -5145,7 +5159,7 @@
         <v>79.42</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>216</v>
       </c>
@@ -5158,14 +5172,14 @@
       <c r="D101" t="s">
         <v>14</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="4">
         <v>2493.2799999999988</v>
       </c>
       <c r="F101">
         <v>0</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -5183,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="M101" s="2">
-        <v>2493.2800000000002</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2808.28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>217</v>
       </c>
@@ -5199,7 +5213,7 @@
       <c r="D102" t="s">
         <v>14</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="4">
         <v>2855.45</v>
       </c>
       <c r="F102">
@@ -5227,7 +5241,7 @@
         <v>2855.45</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>218</v>
       </c>
@@ -5240,7 +5254,7 @@
       <c r="D103" t="s">
         <v>14</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="4">
         <v>622.63</v>
       </c>
       <c r="F103">
@@ -5266,6 +5280,20 @@
       </c>
       <c r="M103" s="2">
         <v>622.63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E104" s="4">
+        <f>SUM(E2:E103)</f>
+        <v>229808.87000000008</v>
+      </c>
+      <c r="M104" s="2">
+        <f>SUM(M2:M103)</f>
+        <v>225849.26000000004</v>
+      </c>
+      <c r="N104" s="3">
+        <f>M104-E104</f>
+        <v>-3959.6100000000442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones funcionalidad movimientos edo cta rutero
</commit_message>
<xml_diff>
--- a/resumen_movimiento_cuenta.xlsx
+++ b/resumen_movimiento_cuenta.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\pruebas\lacteos-doel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B2209-AA1F-446C-876F-A85224D69DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF23E69-349F-42BC-BF4F-A16568CC9ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$103</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
@@ -677,12 +680,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[Blue]#,##0.00;[Red]\(#,##0.00\);[Black]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,13 +695,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -735,21 +729,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1050,16 +1040,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N104"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1113,14 +1105,14 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4">
-        <v>2847.8</v>
+      <c r="E2">
+        <v>3194.86</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1129,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>623.06000000000006</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1154,23 +1146,23 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4">
-        <v>16864.28</v>
+      <c r="E3">
+        <v>17492.150000000001</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5778.7</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>4516.91</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>98.9</v>
+        <v>1251.99</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1179,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>16765.38</v>
+        <v>17501.95</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1195,7 +1187,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>4563.3599999999997</v>
       </c>
       <c r="F4">
@@ -1236,7 +1228,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>1620</v>
       </c>
       <c r="F5">
@@ -1277,7 +1269,7 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>800.18</v>
       </c>
       <c r="F6">
@@ -1318,14 +1310,14 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4">
-        <v>83.229999999999905</v>
+      <c r="E7">
+        <v>122.0899999999999</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>280.25</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1334,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>319.11</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1359,7 +1351,7 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>1883.84</v>
       </c>
       <c r="F8">
@@ -1400,7 +1392,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>1714</v>
       </c>
       <c r="F9">
@@ -1441,7 +1433,7 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>943.79</v>
       </c>
       <c r="F10">
@@ -1482,7 +1474,7 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>2101.3200000000002</v>
       </c>
       <c r="F11">
@@ -1523,7 +1515,7 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12">
         <v>564.79999999999995</v>
       </c>
       <c r="F12">
@@ -1564,7 +1556,7 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13">
         <v>3976.85</v>
       </c>
       <c r="F13">
@@ -1605,29 +1597,29 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="4">
-        <v>1105.77</v>
+      <c r="E14">
+        <v>1110.81</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1056</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>106.02</v>
+        <v>643.05999999999995</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="M14" s="2">
         <v>999.75</v>
@@ -1646,7 +1638,7 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15">
         <v>947.28</v>
       </c>
       <c r="F15">
@@ -1687,7 +1679,7 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16">
         <v>859.56</v>
       </c>
       <c r="F16">
@@ -1728,7 +1720,7 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17">
         <v>-0.46</v>
       </c>
       <c r="F17">
@@ -1769,14 +1761,14 @@
       <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18">
         <v>10.69000000000001</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>109.41</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1794,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>10.69</v>
+        <v>120.1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1810,7 +1802,7 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19">
         <v>183.48</v>
       </c>
       <c r="F19">
@@ -1851,32 +1843,32 @@
       <c r="D20" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="4">
-        <v>4846.1499999999996</v>
+      <c r="E20">
+        <v>5027.6500000000005</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>5133.26</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>4619.2</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>200.61</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="M20" s="2">
-        <v>4846.1499999999996</v>
+        <v>5147.1000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1892,7 +1884,7 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21">
         <v>1055.25</v>
       </c>
       <c r="F21">
@@ -1933,7 +1925,7 @@
       <c r="D22" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22">
         <v>78.41</v>
       </c>
       <c r="F22">
@@ -1974,7 +1966,7 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23">
         <v>368.74</v>
       </c>
       <c r="F23">
@@ -2015,7 +2007,7 @@
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24">
         <v>236.95</v>
       </c>
       <c r="F24">
@@ -2056,17 +2048,17 @@
       <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="4">
-        <v>14402.57</v>
+      <c r="E25">
+        <v>14819.3</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>8443.0400000000009</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>7417.07</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2078,10 +2070,10 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="M25" s="2">
-        <v>14402.57</v>
+        <v>15533.27</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2097,17 +2089,17 @@
       <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="4">
-        <v>9156.2100000000028</v>
+      <c r="E26">
+        <v>8852.8500000000022</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>3846.66</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>3411.3</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2119,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="M26" s="2">
         <v>9156.2099999999991</v>
@@ -2138,7 +2130,7 @@
       <c r="D27" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27">
         <v>2540.7600000000002</v>
       </c>
       <c r="F27">
@@ -2179,7 +2171,7 @@
       <c r="D28" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28">
         <v>2031.85</v>
       </c>
       <c r="F28">
@@ -2220,14 +2212,14 @@
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="4">
-        <v>4990.32</v>
+      <c r="E29">
+        <v>2782.110000000001</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>3387.89</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2236,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1179.68</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2261,7 +2253,7 @@
       <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30">
         <v>1269.5</v>
       </c>
       <c r="F30">
@@ -2302,7 +2294,7 @@
       <c r="D31" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31">
         <v>1071.42</v>
       </c>
       <c r="F31">
@@ -2343,7 +2335,7 @@
       <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32">
         <v>2724.05</v>
       </c>
       <c r="F32">
@@ -2384,7 +2376,7 @@
       <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33">
         <v>307.26</v>
       </c>
       <c r="F33">
@@ -2425,7 +2417,7 @@
       <c r="D34" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34">
         <v>909</v>
       </c>
       <c r="F34">
@@ -2466,14 +2458,14 @@
       <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="4">
-        <v>304.67999999999978</v>
+      <c r="E35">
+        <v>122.1200000000001</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2482,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>81.44</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2507,7 +2499,7 @@
       <c r="D36" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36">
         <v>228.47</v>
       </c>
       <c r="F36">
@@ -2548,7 +2540,7 @@
       <c r="D37" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37">
         <v>159.66999999999999</v>
       </c>
       <c r="F37">
@@ -2589,7 +2581,7 @@
       <c r="D38" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38">
         <v>1660.53</v>
       </c>
       <c r="F38">
@@ -2630,32 +2622,32 @@
       <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="4">
-        <v>-1085.8400000000011</v>
+      <c r="E39">
+        <v>-958.05999999999904</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>2710.02</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1845.08</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>1049.51</v>
+        <v>2450.34</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="M39" s="2">
-        <v>-2135.35</v>
+        <v>-2645.46</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2671,7 +2663,7 @@
       <c r="D40" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40">
         <v>569.36</v>
       </c>
       <c r="F40">
@@ -2712,7 +2704,7 @@
       <c r="D41" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41">
         <v>-2095.84</v>
       </c>
       <c r="F41">
@@ -2753,14 +2745,14 @@
       <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="4">
-        <v>489.18</v>
+      <c r="E42">
+        <v>443.66</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>45.52</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2794,14 +2786,14 @@
       <c r="D43" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="4">
-        <v>-187.8600000000001</v>
+      <c r="E43">
+        <v>-160.24999999999989</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>230.61</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2810,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>75.61</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -2819,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>-187.86</v>
+        <v>-5.25</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2835,7 +2827,7 @@
       <c r="D44" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44">
         <v>53.76</v>
       </c>
       <c r="F44">
@@ -2876,7 +2868,7 @@
       <c r="D45" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45">
         <v>-0.02</v>
       </c>
       <c r="F45">
@@ -2917,7 +2909,7 @@
       <c r="D46" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46">
         <v>683</v>
       </c>
       <c r="F46">
@@ -2958,14 +2950,14 @@
       <c r="D47" t="s">
         <v>14</v>
       </c>
-      <c r="E47" s="4">
-        <v>394.73999999999933</v>
+      <c r="E47">
+        <v>2261.5300000000002</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>775.22</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2974,13 +2966,13 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>2610.0100000000002</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="M47" s="2">
         <v>394.74</v>
@@ -2999,7 +2991,7 @@
       <c r="D48" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48">
         <v>6262.21</v>
       </c>
       <c r="F48">
@@ -3040,7 +3032,7 @@
       <c r="D49" t="s">
         <v>14</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49">
         <v>3661.02</v>
       </c>
       <c r="F49">
@@ -3081,7 +3073,7 @@
       <c r="D50" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50">
         <v>639.80000000000007</v>
       </c>
       <c r="F50">
@@ -3122,32 +3114,32 @@
       <c r="D51" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="4">
-        <v>1770.84</v>
+      <c r="E51">
+        <v>1997.0599999999979</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>2439.4699999999998</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>648</v>
       </c>
       <c r="I51">
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>2000.69</v>
       </c>
       <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="M51" s="2">
-        <v>1770.84</v>
+        <v>1693.84</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3163,7 +3155,7 @@
       <c r="D52" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52">
         <v>127.52</v>
       </c>
       <c r="F52">
@@ -3204,14 +3196,14 @@
       <c r="D53" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="4">
-        <v>6142.72</v>
+      <c r="E53">
+        <v>6460.59</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1691.11</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3220,13 +3212,13 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>1949.98</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="M53" s="2">
         <v>6142.72</v>
@@ -3245,8 +3237,8 @@
       <c r="D54" t="s">
         <v>14</v>
       </c>
-      <c r="E54" s="4">
-        <v>-692.71999999999991</v>
+      <c r="E54">
+        <v>87.280000000000086</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -3261,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>306</v>
+        <v>1086</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -3286,7 +3278,7 @@
       <c r="D55" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55">
         <v>258.99000000000012</v>
       </c>
       <c r="F55">
@@ -3327,7 +3319,7 @@
       <c r="D56" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56">
         <v>349.97</v>
       </c>
       <c r="F56">
@@ -3368,23 +3360,23 @@
       <c r="D57" t="s">
         <v>14</v>
       </c>
-      <c r="E57" s="4">
-        <v>571.19999999999993</v>
+      <c r="E57">
+        <v>25.02</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1524.05</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>951.65</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>26.22</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -3409,7 +3401,7 @@
       <c r="D58" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58">
         <v>2703.54</v>
       </c>
       <c r="F58">
@@ -3450,14 +3442,14 @@
       <c r="D59" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="4">
-        <v>218.42</v>
+      <c r="E59">
+        <v>155.15</v>
       </c>
       <c r="F59">
         <v>0</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>63.27</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3491,14 +3483,14 @@
       <c r="D60" t="s">
         <v>14</v>
       </c>
-      <c r="E60" s="4">
-        <v>68.539999999999793</v>
+      <c r="E60">
+        <v>255.25000000000011</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3507,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>330.71</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -3516,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="2">
-        <v>68.540000000000006</v>
+        <v>236.54</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3532,7 +3524,7 @@
       <c r="D61" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61">
         <v>46.5</v>
       </c>
       <c r="F61">
@@ -3573,7 +3565,7 @@
       <c r="D62" t="s">
         <v>14</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62">
         <v>628.66</v>
       </c>
       <c r="F62">
@@ -3614,7 +3606,7 @@
       <c r="D63" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63">
         <v>6065.4</v>
       </c>
       <c r="F63">
@@ -3655,7 +3647,7 @@
       <c r="D64" t="s">
         <v>14</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64">
         <v>8.27</v>
       </c>
       <c r="F64">
@@ -3696,14 +3688,14 @@
       <c r="D65" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="4">
-        <v>3152.91</v>
+      <c r="E65">
+        <v>3740.98</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3712,13 +3704,13 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>1713.07</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="M65" s="2">
         <v>3152.91</v>
@@ -3737,32 +3729,32 @@
       <c r="D66" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="4">
-        <v>7385.7500000000036</v>
+      <c r="E66">
+        <v>7031.1399999999894</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>18994.32</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>7809.23</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
-        <v>2197.8000000000002</v>
+        <v>8529.2200000000012</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="M66" s="2">
-        <v>5187.95</v>
+        <v>8937.01</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3778,7 +3770,7 @@
       <c r="D67" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67">
         <v>1464.44</v>
       </c>
       <c r="F67">
@@ -3819,23 +3811,23 @@
       <c r="D68" t="s">
         <v>14</v>
       </c>
-      <c r="E68" s="4">
-        <v>-7519.579999999999</v>
+      <c r="E68">
+        <v>-6680.5899999999992</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>2307.84</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>99.61</v>
+        <v>794.06999999999994</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>416.77</v>
+        <v>2456.1999999999998</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -3844,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="2">
-        <v>-8035.96</v>
+        <v>-7623.02</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3860,8 +3852,8 @@
       <c r="D69" t="s">
         <v>14</v>
       </c>
-      <c r="E69" s="4">
-        <v>765.75</v>
+      <c r="E69">
+        <v>1060.8900000000001</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3876,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0</v>
+        <v>295.14</v>
       </c>
       <c r="K69">
         <v>0</v>
@@ -3901,14 +3893,14 @@
       <c r="D70" t="s">
         <v>14</v>
       </c>
-      <c r="E70" s="4">
-        <v>508.61000000000041</v>
+      <c r="E70">
+        <v>136.15000000000029</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>607.61</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3917,13 +3909,13 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>0</v>
+        <v>210.15</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M70" s="2">
         <v>508.61</v>
@@ -3942,14 +3934,14 @@
       <c r="D71" t="s">
         <v>14</v>
       </c>
-      <c r="E71" s="4">
-        <v>-4366.3500000000004</v>
+      <c r="E71">
+        <v>-285.56000000000131</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1197.28</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3958,16 +3950,16 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>0</v>
+        <v>4817.2299999999996</v>
       </c>
       <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="M71" s="2">
-        <v>-4366.3500000000004</v>
+        <v>-4076.51</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3983,7 +3975,7 @@
       <c r="D72" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72">
         <v>332.51</v>
       </c>
       <c r="F72">
@@ -4024,7 +4016,7 @@
       <c r="D73" t="s">
         <v>14</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73">
         <v>-0.45</v>
       </c>
       <c r="F73">
@@ -4065,7 +4057,7 @@
       <c r="D74" t="s">
         <v>14</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74">
         <v>69.7</v>
       </c>
       <c r="F74">
@@ -4106,7 +4098,7 @@
       <c r="D75" t="s">
         <v>14</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75">
         <v>-45.32</v>
       </c>
       <c r="F75">
@@ -4147,17 +4139,17 @@
       <c r="D76" t="s">
         <v>14</v>
       </c>
-      <c r="E76" s="4">
-        <v>15773.34</v>
+      <c r="E76">
+        <v>14778.84</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>2599.35</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>1410.85</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -4169,7 +4161,7 @@
         <v>0</v>
       </c>
       <c r="L76">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="M76" s="2">
         <v>15773.34</v>
@@ -4188,7 +4180,7 @@
       <c r="D77" t="s">
         <v>14</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77">
         <v>146.16999999999999</v>
       </c>
       <c r="F77">
@@ -4229,7 +4221,7 @@
       <c r="D78" t="s">
         <v>14</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78">
         <v>15630.76</v>
       </c>
       <c r="F78">
@@ -4270,7 +4262,7 @@
       <c r="D79" t="s">
         <v>14</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79">
         <v>5474.67</v>
       </c>
       <c r="F79">
@@ -4311,7 +4303,7 @@
       <c r="D80" t="s">
         <v>14</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80">
         <v>200.92</v>
       </c>
       <c r="F80">
@@ -4352,7 +4344,7 @@
       <c r="D81" t="s">
         <v>14</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81">
         <v>664.13</v>
       </c>
       <c r="F81">
@@ -4393,7 +4385,7 @@
       <c r="D82" t="s">
         <v>14</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82">
         <v>-0.01</v>
       </c>
       <c r="F82">
@@ -4434,7 +4426,7 @@
       <c r="D83" t="s">
         <v>14</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83">
         <v>3.01</v>
       </c>
       <c r="F83">
@@ -4475,7 +4467,7 @@
       <c r="D84" t="s">
         <v>14</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84">
         <v>-0.04</v>
       </c>
       <c r="F84">
@@ -4516,32 +4508,32 @@
       <c r="D85" t="s">
         <v>14</v>
       </c>
-      <c r="E85" s="4">
-        <v>17878.04</v>
+      <c r="E85">
+        <v>15621.99</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>7077.79</v>
       </c>
       <c r="G85">
         <v>0</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="I85">
         <v>0</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>2863.85</v>
       </c>
       <c r="K85">
         <v>0</v>
       </c>
       <c r="L85">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="M85" s="2">
-        <v>17878.04</v>
+        <v>18780.93</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4557,7 +4549,7 @@
       <c r="D86" t="s">
         <v>14</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86">
         <v>460.68</v>
       </c>
       <c r="F86">
@@ -4598,7 +4590,7 @@
       <c r="D87" t="s">
         <v>14</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87">
         <v>399.98</v>
       </c>
       <c r="F87">
@@ -4639,32 +4631,32 @@
       <c r="D88" t="s">
         <v>14</v>
       </c>
-      <c r="E88" s="4">
-        <v>1091.79</v>
+      <c r="E88">
+        <v>1672.0800000000011</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>2522.87</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1546.94</v>
       </c>
       <c r="I88">
         <v>0</v>
       </c>
       <c r="J88">
-        <v>0</v>
+        <v>1102.17</v>
       </c>
       <c r="K88">
         <v>0</v>
       </c>
       <c r="L88">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="M88" s="2">
-        <v>1091.79</v>
+        <v>1452.84</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4680,7 +4672,7 @@
       <c r="D89" t="s">
         <v>14</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89">
         <v>243.14</v>
       </c>
       <c r="F89">
@@ -4721,7 +4713,7 @@
       <c r="D90" t="s">
         <v>14</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90">
         <v>1162.33</v>
       </c>
       <c r="F90">
@@ -4762,7 +4754,7 @@
       <c r="D91" t="s">
         <v>14</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91">
         <v>8032.94</v>
       </c>
       <c r="F91">
@@ -4803,7 +4795,7 @@
       <c r="D92" t="s">
         <v>14</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92">
         <v>261.20999999999998</v>
       </c>
       <c r="F92">
@@ -4844,7 +4836,7 @@
       <c r="D93" t="s">
         <v>14</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93">
         <v>24.050000000000072</v>
       </c>
       <c r="F93">
@@ -4885,7 +4877,7 @@
       <c r="D94" t="s">
         <v>14</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94">
         <v>3714.63</v>
       </c>
       <c r="F94">
@@ -4926,7 +4918,7 @@
       <c r="D95" t="s">
         <v>14</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95">
         <v>240.98</v>
       </c>
       <c r="F95">
@@ -4967,7 +4959,7 @@
       <c r="D96" t="s">
         <v>14</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96">
         <v>127.77</v>
       </c>
       <c r="F96">
@@ -4995,7 +4987,7 @@
         <v>127.77</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>206</v>
       </c>
@@ -5008,17 +5000,17 @@
       <c r="D97" t="s">
         <v>14</v>
       </c>
-      <c r="E97" s="4">
-        <v>234.759999999999</v>
+      <c r="E97">
+        <v>446.13000000000068</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>1895.04</v>
       </c>
       <c r="G97">
         <v>0</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1812.93</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -5033,10 +5025,10 @@
         <v>0</v>
       </c>
       <c r="M97" s="2">
-        <v>234.76</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+        <v>528.24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>208</v>
       </c>
@@ -5049,17 +5041,17 @@
       <c r="D98" t="s">
         <v>14</v>
       </c>
-      <c r="E98" s="4">
-        <v>32396.41</v>
+      <c r="E98">
+        <v>32943.980000000003</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>8681.73</v>
       </c>
       <c r="G98">
         <v>0</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>6700.72</v>
       </c>
       <c r="I98">
         <v>0</v>
@@ -5071,13 +5063,13 @@
         <v>0</v>
       </c>
       <c r="L98">
-        <v>0</v>
+        <v>628</v>
       </c>
       <c r="M98" s="2">
-        <v>32396.41</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+        <v>34296.99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>210</v>
       </c>
@@ -5090,14 +5082,14 @@
       <c r="D99" t="s">
         <v>14</v>
       </c>
-      <c r="E99" s="4">
-        <v>785.53999999999985</v>
+      <c r="E99">
+        <v>780.35000000000025</v>
       </c>
       <c r="F99">
         <v>0</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>1171.04</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -5106,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="J99">
-        <v>0</v>
+        <v>925.85</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -5115,10 +5107,10 @@
         <v>0</v>
       </c>
       <c r="M99" s="2">
-        <v>785.54</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1025.54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>214</v>
       </c>
@@ -5131,7 +5123,7 @@
       <c r="D100" t="s">
         <v>14</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E100">
         <v>79.42</v>
       </c>
       <c r="F100">
@@ -5159,7 +5151,7 @@
         <v>79.42</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>216</v>
       </c>
@@ -5172,14 +5164,14 @@
       <c r="D101" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="4">
-        <v>2493.2799999999988</v>
+      <c r="E101">
+        <v>2808.2799999999988</v>
       </c>
       <c r="F101">
         <v>0</v>
       </c>
       <c r="G101">
-        <v>315</v>
+        <v>1260</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -5188,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -5200,7 +5192,7 @@
         <v>2808.28</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>217</v>
       </c>
@@ -5213,14 +5205,14 @@
       <c r="D102" t="s">
         <v>14</v>
       </c>
-      <c r="E102" s="4">
-        <v>2855.45</v>
+      <c r="E102">
+        <v>2915.45</v>
       </c>
       <c r="F102">
         <v>0</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -5229,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="J102">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="K102">
         <v>0</v>
@@ -5241,7 +5233,7 @@
         <v>2855.45</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>218</v>
       </c>
@@ -5254,7 +5246,7 @@
       <c r="D103" t="s">
         <v>14</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103">
         <v>622.63</v>
       </c>
       <c r="F103">
@@ -5282,21 +5274,8 @@
         <v>622.63</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E104" s="4">
-        <f>SUM(E2:E103)</f>
-        <v>229808.87000000008</v>
-      </c>
-      <c r="M104" s="2">
-        <f>SUM(M2:M103)</f>
-        <v>225849.26000000004</v>
-      </c>
-      <c r="N104" s="3">
-        <f>M104-E104</f>
-        <v>-3959.6100000000442</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:M103" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>